<commit_message>
Add calculation of total return
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -503,17 +503,25 @@
         <v>23.55</v>
       </c>
       <c r="E2" t="n">
-        <v>21.60000038146973</v>
-      </c>
-      <c r="F2" t="inlineStr"/>
+        <v>21.6</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.78</v>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>22.06.2023</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>-8.279999999999999</v>
+      </c>
+      <c r="I2" t="n">
+        <v>611.4300000000001</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-4.50106157112526</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -533,17 +541,25 @@
         <v>24.66</v>
       </c>
       <c r="E3" t="n">
-        <v>21.60000038146973</v>
-      </c>
-      <c r="F3" t="inlineStr"/>
+        <v>21.6</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.78</v>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>27.07.2023</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>-12.41</v>
+      </c>
+      <c r="I3" t="n">
+        <v>356</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-8.799675587996749</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -557,23 +573,31 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>100</v>
+        <v>983</v>
       </c>
       <c r="D4" t="n">
-        <v>24.66</v>
+        <v>75.65000000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>75.84999847412109</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
+        <v>75.81999999999999</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.66</v>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>27.07.2024</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+          <t>27.07.2023</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1376.2</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2.075346992729667</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add pivot table with summary per ticker
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stocks" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stock log" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Portfolio Summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,15 +472,25 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Cost Basis</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Market Value</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Capital Gains</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Dividends Paid</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Total Return</t>
         </is>
@@ -503,7 +514,7 @@
         <v>23.55</v>
       </c>
       <c r="E2" t="n">
-        <v>21.6</v>
+        <v>21.53</v>
       </c>
       <c r="F2" t="n">
         <v>1.78</v>
@@ -514,13 +525,19 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>-8.279999999999999</v>
+        <v>16178.85</v>
       </c>
       <c r="I2" t="n">
+        <v>14791.11</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-8.58</v>
+      </c>
+      <c r="K2" t="n">
         <v>611.4300000000001</v>
       </c>
-      <c r="J2" t="n">
-        <v>-4.50106157112526</v>
+      <c r="L2" t="n">
+        <v>-4.99</v>
       </c>
     </row>
     <row r="3">
@@ -541,7 +558,7 @@
         <v>24.66</v>
       </c>
       <c r="E3" t="n">
-        <v>21.6</v>
+        <v>21.53</v>
       </c>
       <c r="F3" t="n">
         <v>1.78</v>
@@ -552,13 +569,19 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>-12.41</v>
+        <v>9864</v>
       </c>
       <c r="I3" t="n">
+        <v>8612</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-12.69</v>
+      </c>
+      <c r="K3" t="n">
         <v>356</v>
       </c>
-      <c r="J3" t="n">
-        <v>-8.799675587996749</v>
+      <c r="L3" t="n">
+        <v>-9.42</v>
       </c>
     </row>
     <row r="4">
@@ -590,13 +613,121 @@
         </is>
       </c>
       <c r="H4" t="n">
+        <v>74363.95000000001</v>
+      </c>
+      <c r="I4" t="n">
+        <v>74531.06</v>
+      </c>
+      <c r="J4" t="n">
         <v>0.22</v>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
         <v>1376.2</v>
       </c>
-      <c r="J4" t="n">
-        <v>2.075346992729667</v>
+      <c r="L4" t="n">
+        <v>2.11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Number of Shares</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cost Basis</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Market Value</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Dividends Paid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Average price paid, USD</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Capital Gains, %</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Total Return, %</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1087</v>
+      </c>
+      <c r="B2" t="n">
+        <v>26042.85</v>
+      </c>
+      <c r="C2" t="n">
+        <v>23403.11</v>
+      </c>
+      <c r="D2" t="n">
+        <v>967.4300000000001</v>
+      </c>
+      <c r="E2" t="n">
+        <v>23.96</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-10.14</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-6.68</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>983</v>
+      </c>
+      <c r="B3" t="n">
+        <v>74363.95000000001</v>
+      </c>
+      <c r="C3" t="n">
+        <v>74531.06</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1376.2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>75.65000000000001</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add cache sqllite for yahoo scrapping to avoid ip ban and speed up the process
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -514,7 +514,7 @@
         <v>23.55</v>
       </c>
       <c r="E2" t="n">
-        <v>21.53</v>
+        <v>21.7</v>
       </c>
       <c r="F2" t="n">
         <v>1.78</v>
@@ -528,16 +528,16 @@
         <v>16178.85</v>
       </c>
       <c r="I2" t="n">
-        <v>14791.11</v>
+        <v>14907.9</v>
       </c>
       <c r="J2" t="n">
-        <v>-8.58</v>
+        <v>-7.86</v>
       </c>
       <c r="K2" t="n">
         <v>611.4300000000001</v>
       </c>
       <c r="L2" t="n">
-        <v>-4.99</v>
+        <v>-4.24</v>
       </c>
     </row>
     <row r="3">
@@ -558,7 +558,7 @@
         <v>24.66</v>
       </c>
       <c r="E3" t="n">
-        <v>21.53</v>
+        <v>21.7</v>
       </c>
       <c r="F3" t="n">
         <v>1.78</v>
@@ -572,16 +572,16 @@
         <v>9864</v>
       </c>
       <c r="I3" t="n">
-        <v>8612</v>
+        <v>8680</v>
       </c>
       <c r="J3" t="n">
-        <v>-12.69</v>
+        <v>-12</v>
       </c>
       <c r="K3" t="n">
         <v>356</v>
       </c>
       <c r="L3" t="n">
-        <v>-9.42</v>
+        <v>-8.710000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -602,7 +602,7 @@
         <v>75.65000000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>75.81999999999999</v>
+        <v>76.23</v>
       </c>
       <c r="F4" t="n">
         <v>2.66</v>
@@ -616,16 +616,16 @@
         <v>74363.95000000001</v>
       </c>
       <c r="I4" t="n">
-        <v>74531.06</v>
+        <v>74934.09000000001</v>
       </c>
       <c r="J4" t="n">
-        <v>0.22</v>
+        <v>0.77</v>
       </c>
       <c r="K4" t="n">
         <v>1376.2</v>
       </c>
       <c r="L4" t="n">
-        <v>2.11</v>
+        <v>2.67</v>
       </c>
     </row>
   </sheetData>
@@ -639,7 +639,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -650,84 +650,99 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Number of Shares</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Cost Basis</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Market Value</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Dividends Paid</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Average price paid, USD</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Capital Gains, %</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Total Return, %</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>AY</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>1087</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>26042.85</v>
       </c>
-      <c r="C2" t="n">
-        <v>23403.11</v>
-      </c>
       <c r="D2" t="n">
+        <v>23587.9</v>
+      </c>
+      <c r="E2" t="n">
         <v>967.4300000000001</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>23.96</v>
       </c>
-      <c r="F2" t="n">
-        <v>-10.14</v>
-      </c>
       <c r="G2" t="n">
-        <v>-6.68</v>
+        <v>-9.43</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-5.94</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>SCHD</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>983</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>74363.95000000001</v>
       </c>
-      <c r="C3" t="n">
-        <v>74531.06</v>
-      </c>
       <c r="D3" t="n">
+        <v>74934.09000000001</v>
+      </c>
+      <c r="E3" t="n">
         <v>1376.2</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>75.65000000000001</v>
       </c>
-      <c r="F3" t="n">
-        <v>0.22</v>
-      </c>
       <c r="G3" t="n">
-        <v>2.11</v>
+        <v>0.77</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add initial support of sell operation
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,50 +447,55 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Operation</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Number of Shares</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Buy Price</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Market Price</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Annual Dividend per Share</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Date of Purchase</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Cost Basis</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Market Value</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Capital Gains</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Dividends Paid</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Total Return</t>
         </is>
@@ -507,36 +512,41 @@
           <t>AY</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>687</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>23.55</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>21.7</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>1.78</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>22.06.2023</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>16178.85</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>14907.9</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>-7.86</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>611.4300000000001</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>-4.24</v>
       </c>
     </row>
@@ -551,36 +561,41 @@
           <t>AY</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>400</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>24.66</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>21.7</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>1.78</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>27.07.2023</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>9864</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>8680</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>-12</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>356</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>-8.710000000000001</v>
       </c>
     </row>
@@ -595,37 +610,91 @@
           <t>SCHD</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>983</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>75.65000000000001</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>76.23</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>2.66</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>27.07.2023</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>74363.95000000001</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>74934.09000000001</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>0.77</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>1376.2</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>2.67</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Atlantica Sustainable Infrastru</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AY</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>-100</v>
+      </c>
+      <c r="E5" t="n">
+        <v>23</v>
+      </c>
+      <c r="F5" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>25.11.2023</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>-2300</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-2170</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-5.65</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-44</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-3.81</v>
       </c>
     </row>
   </sheetData>
@@ -696,25 +765,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1087</v>
+        <v>987</v>
       </c>
       <c r="C2" t="n">
-        <v>26042.85</v>
+        <v>23742.85</v>
       </c>
       <c r="D2" t="n">
-        <v>23587.9</v>
+        <v>21417.9</v>
       </c>
       <c r="E2" t="n">
-        <v>967.4300000000001</v>
+        <v>923.4300000000001</v>
       </c>
       <c r="F2" t="n">
-        <v>23.96</v>
+        <v>24.06</v>
       </c>
       <c r="G2" t="n">
-        <v>-9.43</v>
+        <v>-9.81</v>
       </c>
       <c r="H2" t="n">
-        <v>-5.94</v>
+        <v>-6.14</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Add additional sheet to compare performance of portfolio with some indexes
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stock log" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Portfolio Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Total Return" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -524,7 +525,7 @@
         <v>23.55</v>
       </c>
       <c r="F2" t="n">
-        <v>21.7</v>
+        <v>21.69</v>
       </c>
       <c r="G2" t="n">
         <v>1.78</v>
@@ -538,16 +539,16 @@
         <v>16178.85</v>
       </c>
       <c r="J2" t="n">
-        <v>14907.9</v>
+        <v>14901.03</v>
       </c>
       <c r="K2" t="n">
-        <v>-7.86</v>
+        <v>-7.9</v>
       </c>
       <c r="L2" t="n">
         <v>611.4300000000001</v>
       </c>
       <c r="M2" t="n">
-        <v>-4.24</v>
+        <v>-4.28</v>
       </c>
     </row>
     <row r="3">
@@ -573,7 +574,7 @@
         <v>24.66</v>
       </c>
       <c r="F3" t="n">
-        <v>21.7</v>
+        <v>21.69</v>
       </c>
       <c r="G3" t="n">
         <v>1.78</v>
@@ -587,16 +588,16 @@
         <v>9864</v>
       </c>
       <c r="J3" t="n">
-        <v>8680</v>
+        <v>8676</v>
       </c>
       <c r="K3" t="n">
-        <v>-12</v>
+        <v>-12.04</v>
       </c>
       <c r="L3" t="n">
         <v>356</v>
       </c>
       <c r="M3" t="n">
-        <v>-8.710000000000001</v>
+        <v>-8.75</v>
       </c>
     </row>
     <row r="4">
@@ -622,7 +623,7 @@
         <v>75.65000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>76.23</v>
+        <v>76.28</v>
       </c>
       <c r="G4" t="n">
         <v>2.66</v>
@@ -636,16 +637,16 @@
         <v>74363.95000000001</v>
       </c>
       <c r="J4" t="n">
-        <v>74934.09000000001</v>
+        <v>74983.24000000001</v>
       </c>
       <c r="K4" t="n">
-        <v>0.77</v>
+        <v>0.83</v>
       </c>
       <c r="L4" t="n">
         <v>1376.2</v>
       </c>
       <c r="M4" t="n">
-        <v>2.67</v>
+        <v>2.73</v>
       </c>
     </row>
     <row r="5">
@@ -671,7 +672,7 @@
         <v>23</v>
       </c>
       <c r="F5" t="n">
-        <v>21.7</v>
+        <v>21.69</v>
       </c>
       <c r="G5" t="n">
         <v>1.78</v>
@@ -685,16 +686,16 @@
         <v>-2300</v>
       </c>
       <c r="J5" t="n">
-        <v>-2170</v>
+        <v>-2169</v>
       </c>
       <c r="K5" t="n">
-        <v>-5.65</v>
+        <v>-5.7</v>
       </c>
       <c r="L5" t="n">
         <v>-44</v>
       </c>
       <c r="M5" t="n">
-        <v>-3.81</v>
+        <v>-3.86</v>
       </c>
     </row>
   </sheetData>
@@ -771,7 +772,7 @@
         <v>23742.85</v>
       </c>
       <c r="D2" t="n">
-        <v>21417.9</v>
+        <v>21408.03</v>
       </c>
       <c r="E2" t="n">
         <v>923.4300000000001</v>
@@ -780,10 +781,10 @@
         <v>24.06</v>
       </c>
       <c r="G2" t="n">
-        <v>-9.81</v>
+        <v>-9.85</v>
       </c>
       <c r="H2" t="n">
-        <v>-6.14</v>
+        <v>-6.19</v>
       </c>
     </row>
     <row r="3">
@@ -799,7 +800,7 @@
         <v>74363.95000000001</v>
       </c>
       <c r="D3" t="n">
-        <v>74934.09000000001</v>
+        <v>74983.24000000001</v>
       </c>
       <c r="E3" t="n">
         <v>1376.2</v>
@@ -808,10 +809,94 @@
         <v>75.65000000000001</v>
       </c>
       <c r="G3" t="n">
-        <v>0.77</v>
+        <v>0.83</v>
       </c>
       <c r="H3" t="n">
-        <v>2.67</v>
+        <v>2.73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Portfolio</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Price Return, %</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Total Return, %</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>My Portfolio</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>-1.75</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Global X Super Dividend ETF</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.88</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>S&amp;P 500</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" t="n">
+        <v>26.51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add API rate limiter on calls to the yahoo finance
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -623,7 +623,7 @@
         <v>75.65000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>76.28</v>
+        <v>76.3</v>
       </c>
       <c r="G4" t="n">
         <v>2.66</v>
@@ -637,16 +637,16 @@
         <v>74363.95000000001</v>
       </c>
       <c r="J4" t="n">
-        <v>74983.24000000001</v>
+        <v>75002.89999999999</v>
       </c>
       <c r="K4" t="n">
-        <v>0.83</v>
+        <v>0.86</v>
       </c>
       <c r="L4" t="n">
         <v>1376.2</v>
       </c>
       <c r="M4" t="n">
-        <v>2.73</v>
+        <v>2.76</v>
       </c>
     </row>
     <row r="5">
@@ -800,7 +800,7 @@
         <v>74363.95000000001</v>
       </c>
       <c r="D3" t="n">
-        <v>74983.24000000001</v>
+        <v>75002.89999999999</v>
       </c>
       <c r="E3" t="n">
         <v>1376.2</v>
@@ -809,10 +809,10 @@
         <v>75.65000000000001</v>
       </c>
       <c r="G3" t="n">
-        <v>0.83</v>
+        <v>0.86</v>
       </c>
       <c r="H3" t="n">
-        <v>2.73</v>
+        <v>2.76</v>
       </c>
     </row>
   </sheetData>
@@ -861,10 +861,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-1.75</v>
+        <v>-1.73</v>
       </c>
       <c r="D2" t="n">
-        <v>0.61</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="3">
@@ -877,10 +877,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.88</v>
+        <v>-1.56</v>
       </c>
     </row>
     <row r="4">
@@ -893,10 +893,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>26.51</v>
+        <v>26.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add currency converted to convert foreign currencies to USD
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,50 +453,55 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Currency</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Number of Shares</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Buy Price</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Market Price</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Annual Dividend per Share</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Date of Purchase</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Cost Basis</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Market Value</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Capital Gains</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Dividends Paid</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Total Return</t>
         </is>
@@ -518,36 +523,41 @@
           <t>Buy</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>687</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>23.55</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>21.69</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>1.78</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>22.06.2023</t>
         </is>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>16178.85</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>14901.03</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>-7.9</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>611.4300000000001</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>-4.28</v>
       </c>
     </row>
@@ -567,36 +577,41 @@
           <t>Buy</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>400</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>24.66</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>21.69</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>1.78</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>27.07.2023</t>
         </is>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>9864</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>8676</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>-12.04</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>356</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>-8.75</v>
       </c>
     </row>
@@ -616,36 +631,41 @@
           <t>Buy</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>983</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>75.65000000000001</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>76.3</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>2.66</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>27.07.2023</t>
         </is>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>74363.95000000001</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>75002.89999999999</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>0.86</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>1376.2</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>2.76</v>
       </c>
     </row>
@@ -665,37 +685,96 @@
           <t>Sell</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>-100</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>23</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>21.69</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>1.78</v>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>25.11.2023</t>
         </is>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>-2300</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>-2169</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>-5.7</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>-44</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>-3.86</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ENBRIDGE INC</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ENB.TO</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>CAD</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F6" t="n">
+        <v>45</v>
+      </c>
+      <c r="G6" t="n">
+        <v>35.7825</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>20.05.2023</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>3375</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3578.25</v>
+      </c>
+      <c r="L6" t="n">
+        <v>6.02</v>
+      </c>
+      <c r="M6" t="n">
+        <v>133.5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>10.39</v>
       </c>
     </row>
   </sheetData>
@@ -709,7 +788,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -813,6 +892,34 @@
       </c>
       <c r="H3" t="n">
         <v>2.76</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>ENB.TO</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3375</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3578.25</v>
+      </c>
+      <c r="E4" t="n">
+        <v>133.5</v>
+      </c>
+      <c r="F4" t="n">
+        <v>33.75</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6.01</v>
+      </c>
+      <c r="H4" t="n">
+        <v>10.36</v>
       </c>
     </row>
   </sheetData>
@@ -861,10 +968,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-1.73</v>
+        <v>-1.47</v>
       </c>
       <c r="D2" t="n">
-        <v>0.63</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Update price return for index comparison
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -535,7 +535,7 @@
         <v>23.55</v>
       </c>
       <c r="G2" t="n">
-        <v>21.69</v>
+        <v>21.59</v>
       </c>
       <c r="H2" t="n">
         <v>1.78</v>
@@ -549,16 +549,16 @@
         <v>16178.85</v>
       </c>
       <c r="K2" t="n">
-        <v>14901.03</v>
+        <v>14832.33</v>
       </c>
       <c r="L2" t="n">
-        <v>-7.9</v>
+        <v>-8.32</v>
       </c>
       <c r="M2" t="n">
         <v>611.4300000000001</v>
       </c>
       <c r="N2" t="n">
-        <v>-4.28</v>
+        <v>-4.72</v>
       </c>
     </row>
     <row r="3">
@@ -589,7 +589,7 @@
         <v>24.66</v>
       </c>
       <c r="G3" t="n">
-        <v>21.69</v>
+        <v>21.59</v>
       </c>
       <c r="H3" t="n">
         <v>1.78</v>
@@ -603,16 +603,16 @@
         <v>9864</v>
       </c>
       <c r="K3" t="n">
-        <v>8676</v>
+        <v>8636</v>
       </c>
       <c r="L3" t="n">
-        <v>-12.04</v>
+        <v>-12.45</v>
       </c>
       <c r="M3" t="n">
         <v>356</v>
       </c>
       <c r="N3" t="n">
-        <v>-8.75</v>
+        <v>-9.17</v>
       </c>
     </row>
     <row r="4">
@@ -697,7 +697,7 @@
         <v>23</v>
       </c>
       <c r="G5" t="n">
-        <v>21.69</v>
+        <v>21.59</v>
       </c>
       <c r="H5" t="n">
         <v>1.78</v>
@@ -711,16 +711,16 @@
         <v>-2300</v>
       </c>
       <c r="K5" t="n">
-        <v>-2169</v>
+        <v>-2159</v>
       </c>
       <c r="L5" t="n">
-        <v>-5.7</v>
+        <v>-6.13</v>
       </c>
       <c r="M5" t="n">
         <v>-44</v>
       </c>
       <c r="N5" t="n">
-        <v>-3.86</v>
+        <v>-4.3</v>
       </c>
     </row>
     <row r="6">
@@ -751,7 +751,7 @@
         <v>45</v>
       </c>
       <c r="G6" t="n">
-        <v>35.7825</v>
+        <v>35.73</v>
       </c>
       <c r="H6" t="n">
         <v>3.66</v>
@@ -765,16 +765,16 @@
         <v>3375</v>
       </c>
       <c r="K6" t="n">
-        <v>3578.25</v>
+        <v>3573</v>
       </c>
       <c r="L6" t="n">
-        <v>6.02</v>
+        <v>5.87</v>
       </c>
       <c r="M6" t="n">
         <v>133.5</v>
       </c>
       <c r="N6" t="n">
-        <v>10.39</v>
+        <v>10.23</v>
       </c>
     </row>
   </sheetData>
@@ -851,7 +851,7 @@
         <v>23742.85</v>
       </c>
       <c r="D2" t="n">
-        <v>21408.03</v>
+        <v>21309.33</v>
       </c>
       <c r="E2" t="n">
         <v>923.4300000000001</v>
@@ -860,10 +860,10 @@
         <v>24.06</v>
       </c>
       <c r="G2" t="n">
-        <v>-9.85</v>
+        <v>-10.27</v>
       </c>
       <c r="H2" t="n">
-        <v>-6.19</v>
+        <v>-6.62</v>
       </c>
     </row>
     <row r="3">
@@ -907,7 +907,7 @@
         <v>3375</v>
       </c>
       <c r="D4" t="n">
-        <v>3578.25</v>
+        <v>3573</v>
       </c>
       <c r="E4" t="n">
         <v>133.5</v>
@@ -916,10 +916,10 @@
         <v>33.75</v>
       </c>
       <c r="G4" t="n">
-        <v>6.01</v>
+        <v>5.87</v>
       </c>
       <c r="H4" t="n">
-        <v>10.36</v>
+        <v>10.21</v>
       </c>
     </row>
   </sheetData>
@@ -968,10 +968,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-1.47</v>
+        <v>-1.57</v>
       </c>
       <c r="D2" t="n">
-        <v>0.95</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="3">
@@ -984,7 +984,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>-1.99</v>
       </c>
       <c r="D3" t="n">
         <v>-1.56</v>
@@ -1000,7 +1000,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>25.85</v>
       </c>
       <c r="D4" t="n">
         <v>26.56</v>

</xml_diff>